<commit_message>
Rewrite the "create" page
</commit_message>
<xml_diff>
--- a/create/SleepGraph.xlsx
+++ b/create/SleepGraph.xlsx
@@ -465,13 +465,13 @@
   <dimension ref="A1:AD39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD9" activeCellId="0" sqref="AD9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="2" style="2" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="2" style="2" width="5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="26" style="3" width="8.67"/>
   </cols>
   <sheetData>
@@ -551,7 +551,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
-        <v>36527</v>
+        <v>43832</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="9"/>
@@ -617,7 +617,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
-        <v>36528</v>
+        <v>43833</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -648,7 +648,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>36529</v>
+        <v>43834</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -679,7 +679,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>36530</v>
+        <v>43835</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -710,7 +710,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <v>36531</v>
+        <v>43836</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -741,7 +741,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>36532</v>
+        <v>43837</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -772,7 +772,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>36533</v>
+        <v>43838</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -803,7 +803,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <v>36534</v>
+        <v>43839</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -834,7 +834,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
-        <v>36535</v>
+        <v>43840</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -865,7 +865,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
-        <v>36536</v>
+        <v>43841</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -896,7 +896,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
-        <v>36537</v>
+        <v>43842</v>
       </c>
       <c r="AB13" s="20"/>
       <c r="AC13" s="3" t="s">
@@ -908,7 +908,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
-        <v>36538</v>
+        <v>43843</v>
       </c>
       <c r="AB14" s="21"/>
       <c r="AC14" s="3" t="s">
@@ -920,7 +920,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
-        <v>36539</v>
+        <v>43844</v>
       </c>
       <c r="AB15" s="22"/>
       <c r="AC15" s="3" t="s">
@@ -932,128 +932,128 @@
     </row>
     <row r="16" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
-        <v>36540</v>
+        <v>43845</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
-        <v>36541</v>
+        <v>43846</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
-        <v>36542</v>
+        <v>43847</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <v>36543</v>
+        <v>43848</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <v>36544</v>
+        <v>43849</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <v>36545</v>
+        <v>43850</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <v>36546</v>
+        <v>43851</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <v>36547</v>
+        <v>43852</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <v>36548</v>
+        <v>43853</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
-        <v>36549</v>
+        <v>43854</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <v>36550</v>
+        <v>43855</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <v>36551</v>
+        <v>43856</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
-        <v>36552</v>
+        <v>43857</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
-        <v>36553</v>
+        <v>43858</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
-        <v>36554</v>
+        <v>43859</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
-        <v>36555</v>
+        <v>43860</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
-        <v>36556</v>
+        <v>43861</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
-        <v>36557</v>
+        <v>43862</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
-        <v>36558</v>
+        <v>43863</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="n">
-        <v>36559</v>
+        <v>43864</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
-        <v>36560</v>
+        <v>43865</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
-        <v>36561</v>
+        <v>43866</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
-        <v>36562</v>
+        <v>43867</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
-        <v>36563</v>
+        <v>43868</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>